<commit_message>
Updated the budget with new fan, battery, wiring and LED.
</commit_message>
<xml_diff>
--- a/3 - Project Management/3.1 - Budget/FarmShare Budget.xlsx
+++ b/3 - Project Management/3.1 - Budget/FarmShare Budget.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4500" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="11220" yWindow="4440" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Total Budget" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="85">
   <si>
     <t>Component</t>
   </si>
@@ -71,9 +71,6 @@
     <t>http://www.amazon.com/Renogy-Amp-Solar-Charge-Controller/dp/B00BCTLIHC/ref=sr_1_1?ie=UTF8&amp;qid=1445965383&amp;sr=8-1&amp;keywords=renogy+charge+controller</t>
   </si>
   <si>
-    <t>http://www.amazon.com/VMAX-MB86-50-Replacement-Scooter-Upgrades/dp/B00BJBCZV6/ref=sr_1_1?ie=UTF8&amp;qid=1442094654&amp;sr=8-1&amp;keywords=12V+battery+deep+cycle+40AH</t>
-  </si>
-  <si>
     <t>Switch</t>
   </si>
   <si>
@@ -185,15 +182,9 @@
     <t>See individual budget in "Wiring" tab</t>
   </si>
   <si>
-    <t>http://www.amazon.com/Marine-Electric-Bilge-Blower-130cfm/dp/B00F7ANK7S/ref=sr_1_2?ie=UTF8&amp;qid=1445966228&amp;sr=8-2&amp;keywords=seaflo+blower+3%22</t>
-  </si>
-  <si>
     <t>Fan</t>
   </si>
   <si>
-    <t>12V marine blower, 130CFM, 3" outlet, 2.5A</t>
-  </si>
-  <si>
     <t>Code:</t>
   </si>
   <si>
@@ -216,6 +207,75 @@
   </si>
   <si>
     <t>Cosmetic cover for switches</t>
+  </si>
+  <si>
+    <t>http://www.letsgogreen.com/composting-accessories.html</t>
+  </si>
+  <si>
+    <t>12V fan designed for compostable toilets, 2.4W, preinstalled in 11" of 4" PVC pipe</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/Flexible-Lights-Daylight-Non-waterproof-Lighting/dp/B00HSF65MC/ref=sr_1_1?s=hi&amp;ie=UTF8&amp;qid=1446611279&amp;sr=1-1&amp;keywords=12v+led+light+strip</t>
+  </si>
+  <si>
+    <t>Lighting strip we can cut to desired length, easily connects to 12V power</t>
+  </si>
+  <si>
+    <t>Total (before tax):</t>
+  </si>
+  <si>
+    <t>Tax:</t>
+  </si>
+  <si>
+    <t>Segment</t>
+  </si>
+  <si>
+    <t>Material</t>
+  </si>
+  <si>
+    <t>Gauge</t>
+  </si>
+  <si>
+    <t>Length (ft.)</t>
+  </si>
+  <si>
+    <t>Price / ft.</t>
+  </si>
+  <si>
+    <t>Solar panel to charge controller</t>
+  </si>
+  <si>
+    <t>Copper</t>
+  </si>
+  <si>
+    <t>http://www.lowes.com/pd_72480-295-11587347___?productId=3136843&amp;Ns=p_product_price|0&amp;pl=1&amp;Ntt=awg+12+wire</t>
+  </si>
+  <si>
+    <t>Charge controller to battery</t>
+  </si>
+  <si>
+    <t>Source for wire sizing:</t>
+  </si>
+  <si>
+    <t>http://www.engineeringtoolbox.com/amps-wire-gauge-d_730.html</t>
+  </si>
+  <si>
+    <t>http://www.lowes.com/pd_72529-295-22973201___?productId=3129527&amp;Ns=p_product_price|0&amp;pl=1&amp;Ntt=awg+10+wire</t>
+  </si>
+  <si>
+    <t>(roll)</t>
+  </si>
+  <si>
+    <t>Connection to fan and LED</t>
+  </si>
+  <si>
+    <t>http://www.lowes.com/pd_18748-12704-172213___?productId=3365702&amp;Ns=p_product_price|0&amp;pl=1&amp;Ntt=awg+16+wire</t>
+  </si>
+  <si>
+    <t>Wet Battery, 12V, 14Ah</t>
+  </si>
+  <si>
+    <t>https://www.batterystuff.com/powersports-batteries/sYB14A-A2.html</t>
   </si>
 </sst>
 </file>
@@ -226,7 +286,7 @@
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -268,6 +328,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -292,7 +373,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -302,8 +383,18 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -315,14 +406,33 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -654,10 +764,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -672,22 +782,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="B1" t="s">
+      <c r="A1" s="12"/>
+      <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="12" t="s">
         <v>2</v>
       </c>
     </row>
@@ -709,7 +820,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G2" t="s">
         <v>13</v>
@@ -734,7 +845,7 @@
         <v>114.76</v>
       </c>
       <c r="F3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -765,18 +876,21 @@
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="1">
-        <v>139.99</v>
+      <c r="C5" s="2">
+        <v>54</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>139.99</v>
+        <v>54</v>
+      </c>
+      <c r="F5" t="s">
+        <v>83</v>
       </c>
       <c r="G5" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -784,23 +898,23 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" s="1">
-        <v>21.5</v>
+        <v>53</v>
+      </c>
+      <c r="C6" s="3">
+        <v>50</v>
       </c>
       <c r="D6">
         <v>2</v>
       </c>
       <c r="E6" s="1">
         <f>D6*C6</f>
-        <v>43</v>
+        <v>100</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="G6" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -810,15 +924,21 @@
       <c r="B7" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="2">
-        <v>10</v>
+      <c r="C7" s="3">
+        <v>6.45</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>6.45</v>
+      </c>
+      <c r="F7" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -826,7 +946,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="3">
         <v>0.69</v>
@@ -839,10 +959,10 @@
         <v>1.38</v>
       </c>
       <c r="F8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -850,7 +970,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="1">
         <v>0.39</v>
@@ -863,10 +983,10 @@
         <v>0.78</v>
       </c>
       <c r="F9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -887,10 +1007,10 @@
         <v>11.28</v>
       </c>
       <c r="F10" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -898,7 +1018,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C11" s="3">
         <v>2.1800000000000002</v>
@@ -911,10 +1031,10 @@
         <v>2.1800000000000002</v>
       </c>
       <c r="F11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -924,38 +1044,65 @@
       <c r="B12" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="2">
-        <v>30</v>
+      <c r="C12" s="3">
+        <f>Wiring!G6</f>
+        <v>13.459999999999999</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>13.459999999999999</v>
       </c>
       <c r="F12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="D14" t="s">
-        <v>12</v>
-      </c>
+      <c r="C14" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="11"/>
       <c r="E14" s="1">
         <f>SUM(E2:E12)</f>
-        <v>383.35999999999996</v>
+        <v>334.27999999999992</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="C15" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" s="11"/>
+      <c r="E15" s="1">
+        <f>E14*0.0825</f>
+        <v>27.578099999999996</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="B16" t="s">
-        <v>57</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>58</v>
+      <c r="C16" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="11"/>
+      <c r="E16" s="1">
+        <f>E15+E14</f>
+        <v>361.85809999999992</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="B18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -971,7 +1118,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -985,25 +1132,25 @@
     <col min="7" max="7" width="145" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="4"/>
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:7" s="12" customFormat="1">
+      <c r="A1" s="13"/>
+      <c r="B1" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="14" t="s">
         <v>26</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1011,13 +1158,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" s="5">
         <v>2</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E2" s="6">
         <v>13.32</v>
@@ -1027,7 +1174,7 @@
         <v>26.64</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1035,13 +1182,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" s="5">
         <v>2</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E3" s="6">
         <v>14.98</v>
@@ -1051,7 +1198,7 @@
         <v>29.96</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1059,13 +1206,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="5">
         <v>3</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E4" s="6">
         <v>8.56</v>
@@ -1075,7 +1222,7 @@
         <v>25.68</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1083,13 +1230,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="5">
         <v>4</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E5" s="6">
         <v>6.26</v>
@@ -1099,7 +1246,7 @@
         <v>25.04</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1107,13 +1254,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" s="5">
         <v>4</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E6" s="6">
         <v>0.87</v>
@@ -1123,7 +1270,7 @@
         <v>3.48</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1131,13 +1278,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" s="5">
         <v>4</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E7" s="6">
         <v>0.67</v>
@@ -1147,7 +1294,7 @@
         <v>2.68</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1155,13 +1302,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" s="5">
         <v>4</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E8" s="6">
         <v>0.16</v>
@@ -1171,7 +1318,7 @@
         <v>0.64</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1179,13 +1326,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="5">
         <v>8</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E9" s="6">
         <v>0.08</v>
@@ -1195,7 +1342,7 @@
         <v>0.64</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1243,12 +1390,146 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="102.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="12"/>
+      <c r="B1" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2">
+        <v>12</v>
+      </c>
+      <c r="E2">
+        <v>30</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G2" s="1">
+        <f>F2*E2</f>
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="H2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.49</v>
+      </c>
+      <c r="G3" s="1">
+        <f>F3*E3</f>
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="H3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4">
+        <v>16</v>
+      </c>
+      <c r="E4">
+        <v>20</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="G4" s="1">
+        <v>2.31</v>
+      </c>
+      <c r="H4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="1">
+        <f>SUM(G2:G4)</f>
+        <v>13.459999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="B8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>